<commit_message>
finished the DoSMM for all models and generate summary tables of coefficients and data moments.
</commit_message>
<xml_diff>
--- a/workingfolder/OtherData/CPICQ.xlsx
+++ b/workingfolder/OtherData/CPICQ.xlsx
@@ -1042,7 +1042,7 @@
         <v>42005</v>
       </c>
       <c r="B82">
-        <v>1.738615989685059</v>
+        <v>1.745377659797668</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1050,7 +1050,7 @@
         <v>42095</v>
       </c>
       <c r="B83">
-        <v>1.765494823455811</v>
+        <v>1.777267575263977</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1058,7 +1058,7 @@
         <v>42186</v>
       </c>
       <c r="B84">
-        <v>1.90044641494751</v>
+        <v>1.897096157073975</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1066,7 +1066,7 @@
         <v>42278</v>
       </c>
       <c r="B85">
-        <v>2.097802877426147</v>
+        <v>2.071507215499878</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1074,7 +1074,7 @@
         <v>42370</v>
       </c>
       <c r="B86">
-        <v>2.179538726806641</v>
+        <v>2.163610219955444</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1082,7 +1082,7 @@
         <v>42461</v>
       </c>
       <c r="B87">
-        <v>2.229007244110107</v>
+        <v>2.218834638595581</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1090,7 +1090,7 @@
         <v>42552</v>
       </c>
       <c r="B88">
-        <v>2.22666072845459</v>
+        <v>2.216459274291992</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1098,7 +1098,7 @@
         <v>42644</v>
       </c>
       <c r="B89">
-        <v>2.215363264083862</v>
+        <v>2.213071584701538</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1106,7 +1106,7 @@
         <v>42736</v>
       </c>
       <c r="B90">
-        <v>1.986698389053345</v>
+        <v>2.004358291625977</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1114,7 +1114,7 @@
         <v>42826</v>
       </c>
       <c r="B91">
-        <v>1.720883846282959</v>
+        <v>1.729343056678772</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1122,7 +1122,7 @@
         <v>42917</v>
       </c>
       <c r="B92">
-        <v>1.703371405601501</v>
+        <v>1.680276989936829</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1130,7 +1130,7 @@
         <v>43009</v>
       </c>
       <c r="B93">
-        <v>1.766195178031921</v>
+        <v>1.76869010925293</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1138,7 +1138,7 @@
         <v>43101</v>
       </c>
       <c r="B94">
-        <v>2.101063013076782</v>
+        <v>2.065015554428101</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1146,7 +1146,7 @@
         <v>43191</v>
       </c>
       <c r="B95">
-        <v>2.240066051483154</v>
+        <v>2.267652988433838</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1154,7 +1154,7 @@
         <v>43282</v>
       </c>
       <c r="B96">
-        <v>2.180813312530518</v>
+        <v>2.261080026626587</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1162,7 +1162,7 @@
         <v>43374</v>
       </c>
       <c r="B97">
-        <v>2.213837862014771</v>
+        <v>2.203789710998535</v>
       </c>
     </row>
   </sheetData>

</xml_diff>